<commit_message>
Updated Album.csv and how it inserts values into table
</commit_message>
<xml_diff>
--- a/MusicDatabase/MusicDatabaseNEW/Datasets/Album.csv.xlsx
+++ b/MusicDatabase/MusicDatabaseNEW/Datasets/Album.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oneon\CIS560\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B058567-D879-41A8-B2FC-E282B320DDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E964958C-51E8-49B3-B9F3-B1FD0E8316B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1718" yWindow="1508" windowWidth="19695" windowHeight="12067" xr2:uid="{A9C01051-F52E-421E-A95D-7C0AD7D4CA6B}"/>
+    <workbookView xWindow="1380" yWindow="833" windowWidth="19695" windowHeight="12067" xr2:uid="{A9C01051-F52E-421E-A95D-7C0AD7D4CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,6 +390,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,14 +422,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,12 +748,12 @@
   <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.19921875" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -760,8 +764,8 @@
         <v>43077</v>
       </c>
       <c r="C1" t="str">
-        <f>" (N'" &amp; $A1 &amp; "', '" &amp; $B1 &amp; "'),"</f>
-        <v xml:space="preserve"> (N'Chosen', '43077'),</v>
+        <f>" (N'" &amp; $A1 &amp; "', " &amp; $B1 &amp; "),"</f>
+        <v xml:space="preserve"> (N'Chosen', 43077),</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -772,8 +776,8 @@
         <v>44386</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C65" si="0">" (N'" &amp; $A2 &amp; "', '" &amp; $B2 &amp; "'),"</f>
-        <v xml:space="preserve"> (N'STAY - Single', '44386'),</v>
+        <f t="shared" ref="C2:C65" si="0">" (N'" &amp; $A2 &amp; "', " &amp; $B2 &amp; "),"</f>
+        <v xml:space="preserve"> (N'STAY - Single', 44386),</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -785,7 +789,7 @@
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'SOUR', '44337'),</v>
+        <v xml:space="preserve"> (N'SOUR', 44337),</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -797,7 +801,7 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Bad Habits - Single', '44372'),</v>
+        <v xml:space="preserve"> (N'Bad Habits - Single', 44372),</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -809,7 +813,7 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'INDUSTRY BABY S Single', '44400'),</v>
+        <v xml:space="preserve"> (N'INDUSTRY BABY S Single', 44400),</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
@@ -821,7 +825,7 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'MONTERO (Call Me By Your Name) - Single', '44286'),</v>
+        <v xml:space="preserve"> (N'MONTERO (Call Me By Your Name) - Single', 44286),</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -833,7 +837,7 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Kiss Me More (feat. SZA) - Single', '44295'),</v>
+        <v xml:space="preserve"> (N'Kiss Me More (feat. SZA) - Single', 44295),</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -845,7 +849,7 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Todo De Ti - Single', '44336'),</v>
+        <v xml:space="preserve"> (N'Todo De Ti - Single', 44336),</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -857,7 +861,7 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Yonaguni - Single', '44351'),</v>
+        <v xml:space="preserve"> (N'Yonaguni - Single', 44351),</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -869,7 +873,7 @@
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Teatro d'lra - Vol. I', '44274'),</v>
+        <v xml:space="preserve"> (N'Teatro d'lra - Vol. I', 44274),</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -881,7 +885,7 @@
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Levitating (feat. DaBaby) - Single', '44105'),</v>
+        <v xml:space="preserve"> (N'Levitating (feat. DaBaby) - Single', 44105),</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -893,7 +897,7 @@
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Que Mas Pues? - Single', '44344'),</v>
+        <v xml:space="preserve"> (N'Que Mas Pues? - Single', 44344),</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -905,7 +909,7 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Butter/Permission to Dance - EP', '44386'),</v>
+        <v xml:space="preserve"> (N'Butter/Permission to Dance - EP', 44386),</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -917,7 +921,7 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Justice', '44274'),</v>
+        <v xml:space="preserve"> (N'Justice', 44274),</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
@@ -929,7 +933,7 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Save Your Tears (with Ariana Grande) (Remix) - Single', '44309'),</v>
+        <v xml:space="preserve"> (N'Save Your Tears (with Ariana Grande) (Remix) - Single', 44309),</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -941,7 +945,7 @@
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'AM Remix - Single', '44371'),</v>
+        <v xml:space="preserve"> (N'AM Remix - Single', 44371),</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -953,7 +957,7 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Planet Her', '44372'),</v>
+        <v xml:space="preserve"> (N'Planet Her', 44372),</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -965,7 +969,7 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Volando - Remix - Single', '44385'),</v>
+        <v xml:space="preserve"> (N'Volando - Remix - Single', 44385),</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -977,7 +981,7 @@
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Dreamland', '44050'),</v>
+        <v xml:space="preserve"> (N'Dreamland', 44050),</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -989,7 +993,7 @@
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'After Hours', '43910'),</v>
+        <v xml:space="preserve"> (N'After Hours', 43910),</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1001,7 +1005,7 @@
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Pepas - Single', '44371'),</v>
+        <v xml:space="preserve"> (N'Pepas - Single', 44371),</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1013,7 +1017,7 @@
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Motley Crew - Single', '44386'),</v>
+        <v xml:space="preserve"> (N'Motley Crew - Single', 44386),</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="114" x14ac:dyDescent="0.45">
@@ -1025,7 +1029,7 @@
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Friday (feat. Mufasa &amp; Hypeman) - Dopamine Re-Edit - Single', '44211'),</v>
+        <v xml:space="preserve"> (N'Friday (feat. Mufasa &amp; Hypeman) - Dopamine Re-Edit - Single', 44211),</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1037,7 +1041,7 @@
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Astronaut In The Ocean - Single', '44202'),</v>
+        <v xml:space="preserve"> (N'Astronaut In The Ocean - Single', 44202),</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1049,7 +1053,7 @@
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'An Evening with Silk Sonic', '44260'),</v>
+        <v xml:space="preserve"> (N'An Evening with Silk Sonic', 44260),</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1061,7 +1065,7 @@
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Don't Go Yet - Single', '44400'),</v>
+        <v xml:space="preserve"> (N'Don't Go Yet - Single', 44400),</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1073,7 +1077,7 @@
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Pareja Del Ano - Single', '44302'),</v>
+        <v xml:space="preserve"> (N'Pareja Del Ano - Single', 44302),</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -1085,7 +1089,7 @@
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Fine Line', '43812'),</v>
+        <v xml:space="preserve"> (N'Fine Line', 43812),</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1097,7 +1101,7 @@
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'F*CK LOVE 3+: OVER YOU', '44404'),</v>
+        <v xml:space="preserve"> (N'F*CK LOVE 3+: OVER YOU', 44404),</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1109,7 +1113,7 @@
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Hall of Fame', '44295'),</v>
+        <v xml:space="preserve"> (N'Hall of Fame', 44295),</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1121,7 +1125,7 @@
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'911 - Remix - Single', '44386'),</v>
+        <v xml:space="preserve"> (N'911 - Remix - Single', 44386),</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1133,7 +1137,7 @@
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'EL ULTIMO TOUR DEL MUNDO', '44162'),</v>
+        <v xml:space="preserve"> (N'EL ULTIMO TOUR DEL MUNDO', 44162),</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1145,7 +1149,7 @@
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Mienteme - Single', '44315'),</v>
+        <v xml:space="preserve"> (N'Mienteme - Single', 44315),</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1157,7 +1161,7 @@
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Poblado - Remix - Single', '44365'),</v>
+        <v xml:space="preserve"> (N'Poblado - Remix - Single', 44365),</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -1169,7 +1173,7 @@
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'BE', '44155'),</v>
+        <v xml:space="preserve"> (N'BE', 44155),</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1181,7 +1185,7 @@
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'The Business - Single', '44090'),</v>
+        <v xml:space="preserve"> (N'The Business - Single', 44090),</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
@@ -1193,7 +1197,7 @@
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Heartbreak Anthem (with David Guetta &amp; Little Mix) - Single', '44336'),</v>
+        <v xml:space="preserve"> (N'Heartbreak Anthem (with David Guetta &amp; Little Mix) - Single', 44336),</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
@@ -1205,7 +1209,7 @@
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'El Dorado', '44281'),</v>
+        <v xml:space="preserve"> (N'El Dorado', 44281),</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1217,7 +1221,7 @@
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Entre Nosotros - Single', '44385'),</v>
+        <v xml:space="preserve"> (N'Entre Nosotros - Single', 44385),</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1229,7 +1233,7 @@
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Fiel - Remix - Single', '44362'),</v>
+        <v xml:space="preserve"> (N'Fiel - Remix - Single', 44362),</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1241,7 +1245,7 @@
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Build a Bitch - Single', '44330'),</v>
+        <v xml:space="preserve"> (N'Build a Bitch - Single', 44330),</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
@@ -1253,7 +1257,7 @@
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Nicky Jam: Bzrp Music Sessions, Vol. 41 - Single', '44377'),</v>
+        <v xml:space="preserve"> (N'Nicky Jam: Bzrp Music Sessions, Vol. 41 - Single', 44377),</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1265,7 +1269,7 @@
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Tiroteo - Remix - Single', '44287'),</v>
+        <v xml:space="preserve"> (N'Tiroteo - Remix - Single', 44287),</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1277,7 +1281,7 @@
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Happier Then Ever', '44407'),</v>
+        <v xml:space="preserve"> (N'Happier Then Ever', 44407),</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1289,7 +1293,7 @@
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Rasputin - Single', '44372'),</v>
+        <v xml:space="preserve"> (N'Rasputin - Single', 44372),</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
@@ -1301,7 +1305,7 @@
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Leave Before You Love Me (with Jonas Brothers) - Single', '44337'),</v>
+        <v xml:space="preserve"> (N'Leave Before You Love Me (with Jonas Brothers) - Single', 44337),</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1313,7 +1317,7 @@
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Freaks - Single', '44331'),</v>
+        <v xml:space="preserve"> (N'Freaks - Single', 44331),</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1325,7 +1329,7 @@
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Meu PedaÃ§o de Pecado - Single', '44348'),</v>
+        <v xml:space="preserve"> (N'Meu PedaÃ§o de Pecado - Single', 44348),</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1337,7 +1341,7 @@
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'2/Catorce - Single', '44241'),</v>
+        <v xml:space="preserve"> (N'2/Catorce - Single', 44241),</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
@@ -1349,7 +1353,7 @@
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'JORDI', '44358'),</v>
+        <v xml:space="preserve"> (N'JORDI', 44358),</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
@@ -1361,7 +1365,7 @@
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Human', '44321'),</v>
+        <v xml:space="preserve"> (N'Human', 44321),</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1373,7 +1377,7 @@
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Thot Shit - Single', '44358'),</v>
+        <v xml:space="preserve"> (N'Thot Shit - Single', 44358),</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1385,7 +1389,7 @@
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Your Love (9PM) - Single', '44211'),</v>
+        <v xml:space="preserve"> (N'Your Love (9PM) - Single', 44211),</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1397,7 +1401,7 @@
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Heartbreak Anniversary - Single', '43882'),</v>
+        <v xml:space="preserve"> (N'Heartbreak Anniversary - Single', 43882),</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1409,7 +1413,7 @@
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Future Nostalgia', '43917'),</v>
+        <v xml:space="preserve"> (N'Future Nostalgia', 43917),</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1421,7 +1425,7 @@
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Dinero - Single', '43133'),</v>
+        <v xml:space="preserve"> (N'Dinero - Single', 43133),</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1433,7 +1437,7 @@
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'I Love You.', '41383'),</v>
+        <v xml:space="preserve"> (N'I Love You.', 41383),</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1445,7 +1449,7 @@
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Sobrio - Single', '44385'),</v>
+        <v xml:space="preserve"> (N'Sobrio - Single', 44385),</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
@@ -1457,7 +1461,7 @@
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Divinely Uninspired To A Hellish Extent', '43602'),</v>
+        <v xml:space="preserve"> (N'Divinely Uninspired To A Hellish Extent', 43602),</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1469,7 +1473,7 @@
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Over The Top (feat. Drake) - Single', '44400'),</v>
+        <v xml:space="preserve"> (N'Over The Top (feat. Drake) - Single', 44400),</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1481,7 +1485,7 @@
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'2055 - Single', '44349'),</v>
+        <v xml:space="preserve"> (N'2055 - Single', 44349),</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1493,7 +1497,7 @@
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'2021 Hitazos', '44281'),</v>
+        <v xml:space="preserve"> (N'2021 Hitazos', 44281),</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1505,7 +1509,7 @@
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'La Ultima Promesa', '44329'),</v>
+        <v xml:space="preserve"> (N'La Ultima Promesa', 44329),</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1517,7 +1521,7 @@
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'Love Tonight - Single', '43083'),</v>
+        <v xml:space="preserve"> (N'Love Tonight - Single', 43083),</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1529,7 +1533,7 @@
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (N'ZITTI E BUONI - Single', '44274'),</v>
+        <v xml:space="preserve"> (N'ZITTI E BUONI - Single', 44274),</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
@@ -1540,8 +1544,8 @@
         <v>44169</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C118" si="1">" (N'" &amp; $A66 &amp; "', '" &amp; $B66 &amp; "'),"</f>
-        <v xml:space="preserve"> (N'Sin Miedo (del Amor y Otros Demonios)', '44169'),</v>
+        <f t="shared" ref="C66:C117" si="1">" (N'" &amp; $A66 &amp; "', " &amp; $B66 &amp; "),"</f>
+        <v xml:space="preserve"> (N'Sin Miedo (del Amor y Otros Demonios)', 44169),</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1553,7 +1557,7 @@
       </c>
       <c r="C67" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Botella Tras Botella - Single', '44309'),</v>
+        <v xml:space="preserve"> (N'Botella Tras Botella - Single', 44309),</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1565,7 +1569,7 @@
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Los Legendarios 001', '44231'),</v>
+        <v xml:space="preserve"> (N'Los Legendarios 001', 44231),</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1577,7 +1581,7 @@
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'The Kids Are Coming - EP', '43755'),</v>
+        <v xml:space="preserve"> (N'The Kids Are Coming - EP', 43755),</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1589,7 +1593,7 @@
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Scary Hours 2', '44260'),</v>
+        <v xml:space="preserve"> (N'Scary Hours 2', 44260),</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
@@ -1601,7 +1605,7 @@
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'INSIDE', '44357'),</v>
+        <v xml:space="preserve"> (N'INSIDE', 44357),</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1613,7 +1617,7 @@
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Goosebumps - Remix - Single', '44211'),</v>
+        <v xml:space="preserve"> (N'Goosebumps - Remix - Single', 44211),</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
@@ -1625,7 +1629,7 @@
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Head &amp; Heart (feat. MNEK) - Single', '44015'),</v>
+        <v xml:space="preserve"> (N'Head &amp; Heart (feat. MNEK) - Single', 44015),</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1637,7 +1641,7 @@
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'BED - Single', '44253'),</v>
+        <v xml:space="preserve"> (N'BED - Single', 44253),</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1649,7 +1653,7 @@
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Iko Iko (My Bestie) - Single', '43619'),</v>
+        <v xml:space="preserve"> (N'Iko Iko (My Bestie) - Single', 43619),</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1661,7 +1665,7 @@
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Better Believe - Single', '44399'),</v>
+        <v xml:space="preserve"> (N'Better Believe - Single', 44399),</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1673,7 +1677,7 @@
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Arcade - Single', '43531'),</v>
+        <v xml:space="preserve"> (N'Arcade - Single', 43531),</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1685,7 +1689,7 @@
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Primer Dia de Clases', '44232'),</v>
+        <v xml:space="preserve"> (N'Primer Dia de Clases', 44232),</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
@@ -1697,7 +1701,7 @@
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Positions', '44134'),</v>
+        <v xml:space="preserve"> (N'Positions', 44134),</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1709,7 +1713,7 @@
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Hollywood's Bleeding', '43714'),</v>
+        <v xml:space="preserve"> (N'Hollywood's Bleeding', 43714),</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1721,7 +1725,7 @@
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Blaues Licht - Single', '44393'),</v>
+        <v xml:space="preserve"> (N'Blaues Licht - Single', 44393),</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1733,7 +1737,7 @@
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Ram Pam Pam - Single', '44306'),</v>
+        <v xml:space="preserve"> (N'Ram Pam Pam - Single', 44306),</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
@@ -1745,7 +1749,7 @@
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'JOSE', '44420'),</v>
+        <v xml:space="preserve"> (N'JOSE', 44420),</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
@@ -1757,7 +1761,7 @@
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N't r a n s p a r e n t s o u l feat. Travis Barker - Single', '44313'),</v>
+        <v xml:space="preserve"> (N't r a n s p a r e n t s o u l feat. Travis Barker - Single', 44313),</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1769,7 +1773,7 @@
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'We're All Alone In This Together', '44385'),</v>
+        <v xml:space="preserve"> (N'We're All Alone In This Together', 44385),</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
@@ -1781,7 +1785,7 @@
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Divinely Uninspired To A Hellish Extent (Extended Edition)', '43791'),</v>
+        <v xml:space="preserve"> (N'Divinely Uninspired To A Hellish Extent (Extended Edition)', 43791),</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1793,7 +1797,7 @@
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Reckless - Single', '44351'),</v>
+        <v xml:space="preserve"> (N'Reckless - Single', 44351),</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
@@ -1805,7 +1809,7 @@
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'No Me Conocen (Remix) [con DUKI, Rei &amp; Tiago PZK] - Single', '44363'),</v>
+        <v xml:space="preserve"> (N'No Me Conocen (Remix) [con DUKI, Rei &amp; Tiago PZK] - Single', 44363),</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
@@ -1817,7 +1821,7 @@
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Evolve', '42909'),</v>
+        <v xml:space="preserve"> (N'Evolve', 42909),</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
@@ -1829,7 +1833,7 @@
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Lemonade (feat. Gunna, Don Toliver &amp; NAV) - Single', '44057'),</v>
+        <v xml:space="preserve"> (N'Lemonade (feat. Gunna, Don Toliver &amp; NAV) - Single', 44057),</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1841,7 +1845,7 @@
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Doo-Wops &amp; Hooligans', '40456'),</v>
+        <v xml:space="preserve"> (N'Doo-Wops &amp; Hooligans', 40456),</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1853,7 +1857,7 @@
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Roses - Imanbek Remix - Single', '44155'),</v>
+        <v xml:space="preserve"> (N'Roses - Imanbek Remix - Single', 44155),</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
@@ -1865,7 +1869,7 @@
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'42', '44301'),</v>
+        <v xml:space="preserve"> (N'42', 44301),</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1877,7 +1881,7 @@
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Fulanito - Single', '44350'),</v>
+        <v xml:space="preserve"> (N'Fulanito - Single', 44350),</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1889,7 +1893,7 @@
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Pari­s - Single', '44386'),</v>
+        <v xml:space="preserve"> (N'Pari­s - Single', 44386),</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1901,7 +1905,7 @@
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'lovely (with Khalid) - Single', '43209'),</v>
+        <v xml:space="preserve"> (N'lovely (with Khalid) - Single', 43209),</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
@@ -1913,7 +1917,7 @@
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Sunflower - Spider-Man: Into the Spider-Verse - Single', '43448'),</v>
+        <v xml:space="preserve"> (N'Sunflower - Spider-Man: Into the Spider-Verse - Single', 43448),</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1925,7 +1929,7 @@
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'double take - Single', '43609'),</v>
+        <v xml:space="preserve"> (N'double take - Single', 43609),</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
@@ -1937,7 +1941,7 @@
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Hot Pink', '43776'),</v>
+        <v xml:space="preserve"> (N'Hot Pink', 43776),</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
@@ -1949,7 +1953,7 @@
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'By Your Side (feat. Tom Grennan) - Single', '44351'),</v>
+        <v xml:space="preserve"> (N'By Your Side (feat. Tom Grennan) - Single', 44351),</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1961,7 +1965,7 @@
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'MORENA - Single', '44364'),</v>
+        <v xml:space="preserve"> (N'MORENA - Single', 44364),</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
@@ -1973,7 +1977,7 @@
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Divide', '42797'),</v>
+        <v xml:space="preserve"> (N'Divide', 42797),</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1985,7 +1989,7 @@
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Senorita - Single', '43637'),</v>
+        <v xml:space="preserve"> (N'Senorita - Single', 43637),</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -1997,7 +2001,7 @@
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'2:50 Remix - Single', '44368'),</v>
+        <v xml:space="preserve"> (N'2:50 Remix - Single', 44368),</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -2009,7 +2013,7 @@
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'BLAME IT ON BABY', '43938'),</v>
+        <v xml:space="preserve"> (N'BLAME IT ON BABY', 43938),</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
@@ -2021,7 +2025,7 @@
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Kid Krow', '43910'),</v>
+        <v xml:space="preserve"> (N'Kid Krow', 43910),</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -2033,7 +2037,7 @@
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'you broke me first - Single', '43938'),</v>
+        <v xml:space="preserve"> (N'you broke me first - Single', 43938),</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -2045,7 +2049,7 @@
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'The Days/Nights - EP', '41640'),</v>
+        <v xml:space="preserve"> (N'The Days/Nights - EP', 41640),</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
@@ -2057,7 +2061,7 @@
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Dream Your Life Away (Special Edition)', '41891'),</v>
+        <v xml:space="preserve"> (N'Dream Your Life Away (Special Edition)', 41891),</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -2069,7 +2073,7 @@
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Nevermind', '33507'),</v>
+        <v xml:space="preserve"> (N'Nevermind', 33507),</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -2081,7 +2085,7 @@
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Wiped Out!', '42307'),</v>
+        <v xml:space="preserve"> (N'Wiped Out!', 42307),</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -2093,7 +2097,7 @@
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Eu Tenho A Senha!', '44348'),</v>
+        <v xml:space="preserve"> (N'Eu Tenho A Senha!', 44348),</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
@@ -2105,7 +2109,7 @@
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Miss The Rage (feat. Playboi Carti) - Single', '44323'),</v>
+        <v xml:space="preserve"> (N'Miss The Rage (feat. Playboi Carti) - Single', 44323),</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -2117,7 +2121,7 @@
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'JORDI (Deluxe Edition)', '44358'),</v>
+        <v xml:space="preserve"> (N'JORDI (Deluxe Edition)', 44358),</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -2129,7 +2133,7 @@
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Long Way Down', '41534'),</v>
+        <v xml:space="preserve"> (N'Long Way Down', 41534),</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -2141,7 +2145,7 @@
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Broken Memories - EP', '44316'),</v>
+        <v xml:space="preserve"> (N'Broken Memories - EP', 44316),</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -2153,10 +2157,11 @@
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> (N'Hozier (Bonus Track Version)', '41901'),</v>
+        <v xml:space="preserve"> (N'Hozier (Bonus Track Version)', 41901),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>